<commit_message>
changed the SAM site repository structure
</commit_message>
<xml_diff>
--- a/Documents/Technical/TestUpload/DDAS_Upload_CaseStudy_1.xlsx
+++ b/Documents/Technical/TestUpload/DDAS_Upload_CaseStudy_1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="63">
   <si>
     <t>Project Number</t>
   </si>
@@ -182,6 +182,27 @@
   </si>
   <si>
     <t>0506/0708</t>
+  </si>
+  <si>
+    <t>0000/0011</t>
+  </si>
+  <si>
+    <t>Robert Jones MD</t>
+  </si>
+  <si>
+    <t>Robert</t>
+  </si>
+  <si>
+    <t>Jones</t>
+  </si>
+  <si>
+    <t>St John's</t>
+  </si>
+  <si>
+    <t>Bangalore</t>
+  </si>
+  <si>
+    <t>India</t>
   </si>
 </sst>
 </file>
@@ -586,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI9"/>
+  <dimension ref="A1:AI10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,6 +883,32 @@
         <v>39</v>
       </c>
     </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" t="s">
+        <v>58</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="J10" t="s">
+        <v>60</v>
+      </c>
+      <c r="K10" t="s">
+        <v>61</v>
+      </c>
+      <c r="P10" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
1. App data downloads folder has new folders created for each site which downloads data files 2. Set up is modified accordingly to create the required files in App data downloads folder 3. New case studies have been created under Documents/Technical/TestUpload 4. Bug - FDAWarningsLetters site was not updating the DataExtractionSucceeded and DataExtractionRequired. This bug is fixed 5. Added FDAWarningsLetter and Disqualification proceedings enums while fetching/retrieving data extraction history for each site 6. Added 'Institute' tab
</commit_message>
<xml_diff>
--- a/Documents/Technical/TestUpload/DDAS_Upload_CaseStudy_1.xlsx
+++ b/Documents/Technical/TestUpload/DDAS_Upload_CaseStudy_1.xlsx
@@ -279,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -287,24 +287,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -607,16 +621,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI10"/>
+  <dimension ref="A1:X11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
@@ -652,17 +666,17 @@
     <col min="35" max="35" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -705,192 +719,181 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="10"/>
+      <c r="I2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="8">
+        <v>889</v>
+      </c>
+      <c r="P2" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
-      <c r="D3" t="s">
-        <v>44</v>
+      <c r="B3" s="4"/>
+      <c r="D3" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="G3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>47</v>
+      <c r="B4" s="4"/>
+      <c r="D4" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="G4" t="s">
-        <v>48</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>50</v>
+      <c r="D5" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="G5" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="H5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="5"/>
-      <c r="I6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O6" s="2">
-        <v>889</v>
-      </c>
-      <c r="P6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
-      <c r="V6" s="2"/>
-      <c r="W6" s="2"/>
-      <c r="X6" s="2"/>
-      <c r="Y6" s="4"/>
-      <c r="Z6" s="4"/>
-      <c r="AA6" s="4"/>
-      <c r="AB6" s="4"/>
-      <c r="AC6" s="4"/>
-      <c r="AD6" s="4"/>
-      <c r="AE6" s="4"/>
-      <c r="AF6" s="4"/>
-      <c r="AG6" s="4"/>
-      <c r="AH6" s="4"/>
-      <c r="AI6" s="4"/>
-    </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="D7" t="s">
-        <v>28</v>
+      <c r="D7" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="G7" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="D8" t="s">
-        <v>33</v>
+      <c r="D8" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="G8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
-      <c r="D9" t="s">
-        <v>36</v>
+      <c r="D9" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="G9" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="H9" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="5" t="s">
         <v>57</v>
       </c>
       <c r="G10" t="s">
@@ -908,6 +911,9 @@
       <c r="P10" t="s">
         <v>62</v>
       </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="D11" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Insitute Findings, Publish related changes
</commit_message>
<xml_diff>
--- a/Documents/Technical/TestUpload/DDAS_Upload_CaseStudy_1.xlsx
+++ b/Documents/Technical/TestUpload/DDAS_Upload_CaseStudy_1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -97,9 +97,6 @@
     <t>US</t>
   </si>
   <si>
-    <t>USA</t>
-  </si>
-  <si>
     <t xml:space="preserve">brown, malcolm d </t>
   </si>
   <si>
@@ -184,9 +181,6 @@
     <t>0506/0708</t>
   </si>
   <si>
-    <t>0000/0011</t>
-  </si>
-  <si>
     <t>Robert Jones MD</t>
   </si>
   <si>
@@ -202,7 +196,13 @@
     <t>Bangalore</t>
   </si>
   <si>
-    <t>India</t>
+    <t>9002/0011</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>BELGIUM</t>
   </si>
 </sst>
 </file>
@@ -623,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,7 +724,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="4" t="s">
@@ -758,7 +758,7 @@
         <v>889</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="Q2" s="8" t="s">
         <v>18</v>
@@ -773,52 +773,52 @@
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="4"/>
       <c r="D3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" t="s">
         <v>28</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="8" t="s">
-        <v>30</v>
-      </c>
       <c r="Q3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="4"/>
       <c r="D4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" t="s">
         <v>33</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" s="8" t="s">
         <v>34</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" t="s">
         <v>36</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>37</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" s="9" t="s">
         <v>38</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -826,64 +826,64 @@
         <v>17</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" t="s">
         <v>40</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="Q6" t="s">
         <v>42</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" t="s">
         <v>44</v>
       </c>
-      <c r="G7" t="s">
+      <c r="I7" s="9" t="s">
         <v>45</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" t="s">
         <v>47</v>
       </c>
-      <c r="G8" t="s">
+      <c r="I8" s="9" t="s">
         <v>48</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" t="s">
         <v>50</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>51</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" s="9" t="s">
         <v>52</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
@@ -891,25 +891,25 @@
         <v>17</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="I10" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="G10" t="s">
+      <c r="J10" t="s">
         <v>58</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="K10" t="s">
         <v>59</v>
       </c>
-      <c r="J10" t="s">
-        <v>60</v>
-      </c>
-      <c r="K10" t="s">
+      <c r="P10" t="s">
         <v>61</v>
-      </c>
-      <c r="P10" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
commit from prev pull
</commit_message>
<xml_diff>
--- a/Documents/Technical/TestUpload/DDAS_Upload_CaseStudy_1.xlsx
+++ b/Documents/Technical/TestUpload/DDAS_Upload_CaseStudy_1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="63">
   <si>
     <t>Project Number</t>
   </si>
@@ -200,6 +200,9 @@
   </si>
   <si>
     <t>USA</t>
+  </si>
+  <si>
+    <t>Project Number 2</t>
   </si>
 </sst>
 </file>
@@ -276,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -317,6 +320,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -618,297 +622,304 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X11"/>
+  <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.28515625" customWidth="1"/>
-    <col min="21" max="21" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.5703125" customWidth="1"/>
-    <col min="24" max="24" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.28515625" customWidth="1"/>
+    <col min="22" max="22" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.5703125" customWidth="1"/>
+    <col min="25" max="25" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>57</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>58</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="7"/>
       <c r="F2" s="7"/>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="7"/>
+      <c r="H2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="10"/>
+      <c r="J2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="K2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="L2" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="L2" s="8"/>
-      <c r="M2" s="11" t="s">
+      <c r="M2" s="8"/>
+      <c r="N2" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="O2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="8">
+      <c r="P2" s="8">
         <v>889245</v>
       </c>
-      <c r="P2" s="12" t="s">
+      <c r="Q2" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="R2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="8"/>
       <c r="S2" s="8"/>
       <c r="T2" s="8"/>
       <c r="U2" s="8"/>
       <c r="V2" s="8"/>
       <c r="W2" s="8"/>
       <c r="X2" s="8"/>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y2" s="8"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>59</v>
       </c>
       <c r="B3" s="4"/>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="4"/>
+      <c r="E3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="J3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="R3" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>59</v>
       </c>
       <c r="B4" s="4"/>
-      <c r="D4" s="5" t="s">
+      <c r="C4" s="4"/>
+      <c r="E4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="J4" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>31</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>32</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="J5" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>58</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>35</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="J6" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>59</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="J7" s="9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>59</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>42</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="J8" s="9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>45</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>46</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="J9" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>58</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>51</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="J10" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>53</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>54</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="D11" s="5"/>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="E11" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>